<commit_message>
phone survey available after 3 weeks and some textual changes
</commit_message>
<xml_diff>
--- a/app/static/csv/eeg.xlsx
+++ b/app/static/csv/eeg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\ruchella\agestudy\app\static\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24288497-930D-49D6-B234-95EC396A7729}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3C2E39-7395-4BD0-B425-A8E97E2B19DF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -346,23 +346,23 @@
     <t xml:space="preserve">Waar zal de EEG test plaatsvinden? </t>
   </si>
   <si>
+    <t xml:space="preserve">EEG tests will occur at the &lt;a href=\contact&gt;Pieter de la Court building of Leiden University (Wassenaarseweg 52, 2333 AK Leiden)&lt;/a&gt;. </t>
+  </si>
+  <si>
+    <t>De EEG metingen zullen plaatsvinden in het  &lt;a href=/contact&gt;Pieder de la Court gebouw van Universiteit Leiden plaatsvinden (Wassenaarseweg 52, 2333 AK Leiden)&lt;/a&gt;. </t>
+  </si>
+  <si>
+    <t>p9</t>
+  </si>
+  <si>
+    <t>Vanwege de huidige geïmplementeerde regels met betrekking tot de COVID-19 crisis, zullen wij alleen EEG experimenten inroosteren als dit weer is toegestaan.</t>
+  </si>
+  <si>
+    <t>Due to the current regulations implemented in regard to the COVID-19 crisis, we will only schedule EEG experiments once it is permitted to do so</t>
+  </si>
+  <si>
     <t xml:space="preserve">Probeer uw smartphone opgeladen te houden en breng ook uw eigen 
-oplader mee om er zeker van tte zijn dat u genoeg </t>
-  </si>
-  <si>
-    <t xml:space="preserve">EEG tests will occur at the &lt;a href=\contact&gt;Pieter de la Court building of Leiden University (Wassenaarseweg 52, 2333 AK Leiden)&lt;/a&gt;. </t>
-  </si>
-  <si>
-    <t>De EEG metingen zullen plaatsvinden in het  &lt;a href=/contact&gt;Pieder de la Court gebouw van Universiteit Leiden plaatsvinden (Wassenaarseweg 52, 2333 AK Leiden)&lt;/a&gt;. </t>
-  </si>
-  <si>
-    <t>p9</t>
-  </si>
-  <si>
-    <t>Vanwege de huidige geïmplementeerde regels met betrekking tot de COVID-19 crisis, zullen wij alleen EEG experimenten inroosteren als dit weer is toegestaan.</t>
-  </si>
-  <si>
-    <t>Due to the current regulations implemented in regard to the COVID-19 crisis, we will only schedule EEG experiments once it is permitted to do so</t>
+oplader mee om er zeker van te zijn dat u genoeg </t>
   </si>
 </sst>
 </file>
@@ -1246,13 +1246,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="C14" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="110.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -1387,7 +1388,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="87" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1442,7 +1443,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="232" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -1450,7 +1451,7 @@
         <v>40</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -1579,21 +1580,21 @@
         <v>84</v>
       </c>
       <c r="B30" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" t="s">
         <v>90</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C31" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>